<commit_message>
Adding is.useful column to phi_constants.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/phi_constants.xlsx
+++ b/inst/extdata/phi_constants.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89A13EB-2A28-564A-A6E9-B8A935CE879B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="460" windowWidth="20020" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17085" yWindow="465" windowWidth="20025" windowHeight="11280"/>
   </bookViews>
   <sheets>
     <sheet name="phi_constants" sheetId="1" r:id="rId1"/>
     <sheet name="temp_calcs" sheetId="2" r:id="rId2"/>
     <sheet name="Serrenho_2013" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
   <si>
     <t>source</t>
   </si>
@@ -66,9 +65,6 @@
     <t>MTH.300.C</t>
   </si>
   <si>
-    <t>LTC.10.C</t>
-  </si>
-  <si>
     <t>T_0 [C]</t>
   </si>
   <si>
@@ -352,12 +348,15 @@
   </si>
   <si>
     <t>LTH.20.C</t>
+  </si>
+  <si>
+    <t>is.useful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -758,76 +757,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="5"/>
+    <col min="2" max="2" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="9">
         <v>0.95599999999999996</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -835,23 +853,29 @@
         <f>temp_calcs!G2</f>
         <v>0.8467020793849932</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9">
         <f>temp_calcs!G3</f>
         <v>0.81746813717700162</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -859,11 +883,14 @@
         <f>temp_calcs!G4</f>
         <v>0.77445705533519227</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -871,35 +898,44 @@
         <f>temp_calcs!G5</f>
         <v>0.7671410615091433</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="9">
         <f>temp_calcs!G6</f>
         <v>0.74433512887860043</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="9">
         <f>temp_calcs!G7</f>
         <v>0.6711332531638321</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -907,11 +943,14 @@
         <f>temp_calcs!G8</f>
         <v>0.57342345688182428</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -919,11 +958,14 @@
         <f>temp_calcs!G9</f>
         <v>0.49899677222367622</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
@@ -931,11 +973,14 @@
         <f>temp_calcs!G10</f>
         <v>0.39311000739723134</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -943,79 +988,100 @@
         <f>temp_calcs!G11</f>
         <v>0.23047032024654968</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="9">
         <f>temp_calcs!G12</f>
         <v>0.13807594176797244</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="9">
         <f>temp_calcs!G13</f>
         <v>5.116834385127067E-2</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="9">
         <f>temp_calcs!G14</f>
         <v>3.4112229234180447E-2</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B20" s="9">
         <f>temp_calcs!G15</f>
-        <v>7.0633939607981588E-2</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+        <v>0.114003420102603</v>
+      </c>
+      <c r="C20" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="9">
-        <f>temp_calcs!G16</f>
-        <v>0.114003420102603</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B2</f>
+        <v>1.06</v>
+      </c>
+      <c r="C22" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1023,51 +1089,66 @@
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="9">
-        <f>Serrenho_2013!B2</f>
-        <v>1.06</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C24" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C27" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1075,11 +1156,14 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1087,11 +1171,14 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>33</v>
       </c>
@@ -1099,11 +1186,14 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>34</v>
       </c>
@@ -1111,11 +1201,14 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>35</v>
       </c>
@@ -1123,11 +1216,14 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>36</v>
       </c>
@@ -1135,23 +1231,29 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B4</f>
+        <v>1.05</v>
+      </c>
+      <c r="C34" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1159,31 +1261,40 @@
         <f>Serrenho_2013!B4</f>
         <v>1.05</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="9">
-        <f>Serrenho_2013!B4</f>
-        <v>1.05</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B5</f>
+        <v>1.04</v>
+      </c>
+      <c r="C37" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>41</v>
       </c>
@@ -1191,11 +1302,14 @@
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>42</v>
       </c>
@@ -1203,11 +1317,14 @@
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>43</v>
       </c>
@@ -1215,115 +1332,148 @@
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C41" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="9">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="9">
+      <c r="C45" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="9">
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C46" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="9">
+        <f>Serrenho_2013!B4</f>
+        <v>1.05</v>
+      </c>
+      <c r="C47" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="9">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="9">
-        <f>Serrenho_2013!B5</f>
-        <v>1.04</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="9">
-        <f>Serrenho_2013!B4</f>
-        <v>1.05</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="9">
+        <v>1</v>
+      </c>
+      <c r="C49" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="9">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>54</v>
       </c>
@@ -1331,99 +1481,126 @@
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B52" s="9">
-        <f>Serrenho_2013!B3</f>
+        <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B53" s="9">
-        <f>Serrenho_2013!B2</f>
-        <v>1.06</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C53" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="9">
+        <f>Serrenho_2013!B9</f>
+        <v>0.6</v>
+      </c>
+      <c r="C55" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="9">
+      <c r="C56" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="9">
         <f>Serrenho_2013!B9</f>
         <v>0.6</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="9">
+      <c r="C57" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="9">
-        <f>Serrenho_2013!B9</f>
-        <v>0.6</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>63</v>
       </c>
@@ -1431,87 +1608,111 @@
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C61" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="9">
+        <f>Serrenho_2013!B5</f>
+        <v>1.04</v>
+      </c>
+      <c r="C62" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C63" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="9">
-        <f>Serrenho_2013!B5</f>
-        <v>1.04</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="9">
+        <v>1</v>
+      </c>
+      <c r="C65" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="9">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>71</v>
       </c>
@@ -1519,75 +1720,96 @@
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="9">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="9">
+        <v>1</v>
+      </c>
+      <c r="C70" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B72" s="9">
+        <f>Serrenho_2013!B10</f>
+        <v>0.25</v>
+      </c>
+      <c r="C72" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" s="9">
-        <f>Serrenho_2013!B10</f>
-        <v>0.25</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B2</f>
+        <v>1.06</v>
+      </c>
+      <c r="C74" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>78</v>
       </c>
@@ -1595,11 +1817,14 @@
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>79</v>
       </c>
@@ -1607,11 +1832,14 @@
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>80</v>
       </c>
@@ -1619,11 +1847,14 @@
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>81</v>
       </c>
@@ -1631,92 +1862,104 @@
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B79" s="9">
-        <f>Serrenho_2013!B2</f>
-        <v>1.06</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C79" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B5</f>
+        <v>1.04</v>
+      </c>
+      <c r="C80" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="9">
-        <f>Serrenho_2013!B5</f>
-        <v>1.04</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C82" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C83" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="9">
+        <v>1</v>
+      </c>
+      <c r="C84" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B86" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>103</v>
+      <c r="C85" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1725,48 +1968,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="68.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="68.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1774,7 +2017,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1">
         <v>1600</v>
@@ -1792,25 +2035,25 @@
         <v>0.8467020793849932</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1">
         <v>1300</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E16" si="0">B3+273.15</f>
+        <f t="shared" ref="E3:E15" si="0">B3+273.15</f>
         <v>287.14999999999998</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F16" si="1">D3+273.15</f>
+        <f t="shared" ref="F3:F15" si="1">D3+273.15</f>
         <v>1573.15</v>
       </c>
       <c r="G3" s="1">
@@ -1818,7 +2061,7 @@
         <v>0.81746813717700162</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +2069,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1">
         <v>1000</v>
@@ -1844,7 +2087,7 @@
         <v>0.77445705533519227</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1852,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1">
         <v>960</v>
@@ -1870,15 +2113,15 @@
         <v>0.7671410615091433</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1">
         <v>850</v>
@@ -1896,15 +2139,15 @@
         <v>0.74433512887860043</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1">
         <v>600</v>
@@ -1922,7 +2165,7 @@
         <v>0.6711332531638321</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +2173,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1">
         <v>400</v>
@@ -1948,7 +2191,7 @@
         <v>0.57342345688182428</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -1956,7 +2199,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1">
         <v>300</v>
@@ -1974,7 +2217,7 @@
         <v>0.49899677222367622</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1982,7 +2225,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1">
         <v>200</v>
@@ -2000,7 +2243,7 @@
         <v>0.39311000739723134</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -2008,7 +2251,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1">
         <v>100</v>
@@ -2026,18 +2269,18 @@
         <v>0.23047032024654968</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1">
         <v>60</v>
@@ -2055,15 +2298,15 @@
         <v>0.13807594176797244</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" s="1">
         <v>20</v>
@@ -2081,18 +2324,18 @@
         <v>5.116834385127067E-2</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1">
         <v>20</v>
@@ -2110,55 +2353,29 @@
         <v>3.4112229234180447E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D15" s="1">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>303.14999999999998</v>
+        <v>293.14999999999998</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>283.14999999999998</v>
+        <v>263.14999999999998</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G16" si="3">(E15/F15)-1</f>
-        <v>7.0633939607981588E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="1">
-        <v>-10</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>263.14999999999998</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G15" si="3">(E15/F15)-1</f>
         <v>0.114003420102603</v>
       </c>
     </row>
@@ -2169,97 +2386,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="J1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1">
         <v>1.06</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1">
         <v>1.06</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1">
         <v>1.04</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1">
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="B9" s="1">
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1">
         <v>0.25</v>

</xml_diff>

<commit_message>
Non-energy use is back to a useful product.
</commit_message>
<xml_diff>
--- a/inst/extdata/phi_constants.xlsx
+++ b/inst/extdata/phi_constants.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71625F49-76C4-1041-A163-D2EA045BA8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA82CC98-4510-0347-83AF-582ABECDEE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="460" windowWidth="20020" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8780" yWindow="460" windowWidth="20020" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phi_constants" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1064,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add rows to phi_constants
</commit_message>
<xml_diff>
--- a/inst/extdata/phi_constants.xlsx
+++ b/inst/extdata/phi_constants.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C37CCD-BBB6-D046-94C0-C775B507C423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522853A1-903F-F74F-ACA5-2E8B26C4CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="460" windowWidth="20020" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24440" yWindow="1000" windowWidth="20020" windowHeight="27280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phi_constants" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
   <si>
     <t>source</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>NEU</t>
+  </si>
+  <si>
+    <t>Resources [of Hydro]</t>
+  </si>
+  <si>
+    <t>Resources [of Primary solid biofuels]</t>
   </si>
 </sst>
 </file>
@@ -766,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B47" sqref="B47:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1138,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1143,22 +1149,18 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="C27" s="9" t="b">
         <v>0</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1173,7 +1175,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1188,7 +1190,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1203,7 +1205,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1218,7 +1220,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1233,7 +1235,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1248,11 +1250,11 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="9">
-        <f>Serrenho_2013!B4</f>
-        <v>1.05</v>
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
       </c>
       <c r="C34" s="9" t="b">
         <v>0</v>
@@ -1263,7 +1265,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="9">
         <f>Serrenho_2013!B4</f>
@@ -1278,33 +1280,33 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="9">
-        <v>1</v>
+        <f>Serrenho_2013!B4</f>
+        <v>1.05</v>
       </c>
       <c r="C36" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="9">
-        <f>Serrenho_2013!B5</f>
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="C37" s="9" t="b">
         <v>0</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="9">
         <f>Serrenho_2013!B5</f>
@@ -1319,7 +1321,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="9">
         <f>Serrenho_2013!B5</f>
@@ -1334,7 +1336,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="9">
         <f>Serrenho_2013!B5</f>
@@ -1349,33 +1351,37 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="9">
+        <f>Serrenho_2013!B5</f>
+        <v>1.04</v>
+      </c>
+      <c r="C41" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B42" s="9">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C41" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="9">
-        <v>1</v>
-      </c>
       <c r="C42" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="9">
         <v>1</v>
@@ -1386,7 +1392,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
@@ -1397,78 +1403,78 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B46" s="9">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C45" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="C46" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B47" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C46" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="C47" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="9">
+        <f>Serrenho_2013!B7</f>
+        <v>1</v>
+      </c>
+      <c r="C48" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B49" s="9">
         <f>Serrenho_2013!B4</f>
         <v>1.05</v>
       </c>
-      <c r="C47" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C48" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="9">
-        <v>1</v>
-      </c>
       <c r="C49" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1483,68 +1489,68 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" s="9">
+        <v>1</v>
+      </c>
+      <c r="C51" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="9">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C51" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="C52" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C53" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B54" s="9">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C52" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="C54" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B55" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C53" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="9">
-        <v>1</v>
-      </c>
-      <c r="C54" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="9">
-        <f>Serrenho_2013!B9</f>
-        <v>0.6</v>
-      </c>
       <c r="C55" s="9" t="b">
         <v>0</v>
       </c>
@@ -1554,22 +1560,18 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
+        <v>1</v>
       </c>
       <c r="C56" s="9" t="b">
         <v>0</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="9">
         <f>Serrenho_2013!B9</f>
@@ -1584,68 +1586,68 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" s="9">
-        <v>1</v>
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C58" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="9">
+        <f>Serrenho_2013!B9</f>
+        <v>0.6</v>
+      </c>
+      <c r="C59" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1</v>
+      </c>
+      <c r="C60" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B61" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C59" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="C61" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B62" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C60" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="9">
-        <f>Serrenho_2013!B3</f>
-        <v>1.06</v>
-      </c>
-      <c r="C61" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="9">
-        <f>Serrenho_2013!B5</f>
-        <v>1.04</v>
-      </c>
       <c r="C62" s="9" t="b">
         <v>0</v>
       </c>
@@ -1655,7 +1657,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" s="9">
         <f>Serrenho_2013!B3</f>
@@ -1670,126 +1672,126 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="9">
+        <f>Serrenho_2013!B5</f>
+        <v>1.04</v>
+      </c>
+      <c r="C64" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="9">
+        <f>Serrenho_2013!B3</f>
+        <v>1.06</v>
+      </c>
+      <c r="C65" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B66" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C64" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B65" s="9">
-        <v>1</v>
-      </c>
-      <c r="C65" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="9">
-        <v>1</v>
-      </c>
       <c r="C66" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="9">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="9">
+        <v>1</v>
+      </c>
+      <c r="C68" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B69" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C67" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+      <c r="C69" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B70" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C68" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69" s="9">
-        <v>1</v>
-      </c>
-      <c r="C69" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" s="9">
-        <v>1</v>
-      </c>
       <c r="C70" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" s="9">
-        <f>Serrenho_2013!B6</f>
-        <v>1.1100000000000001</v>
+        <v>1</v>
       </c>
       <c r="C71" s="9" t="b">
         <v>0</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72" s="9">
-        <f>Serrenho_2013!B10</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C72" s="9" t="b">
         <v>0</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73" s="9">
         <f>Serrenho_2013!B6</f>
@@ -1804,11 +1806,11 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74" s="9">
-        <f>Serrenho_2013!B2</f>
-        <v>1.06</v>
+        <f>Serrenho_2013!B10</f>
+        <v>0.25</v>
       </c>
       <c r="C74" s="9" t="b">
         <v>0</v>
@@ -1819,11 +1821,11 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" s="9">
-        <f>Serrenho_2013!B2</f>
-        <v>1.06</v>
+        <f>Serrenho_2013!B6</f>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C75" s="9" t="b">
         <v>0</v>
@@ -1834,7 +1836,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" s="9">
         <f>Serrenho_2013!B2</f>
@@ -1849,7 +1851,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" s="9">
         <f>Serrenho_2013!B2</f>
@@ -1864,7 +1866,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B78" s="9">
         <f>Serrenho_2013!B2</f>
@@ -1879,94 +1881,124 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B79" s="9">
-        <v>1</v>
+        <f>Serrenho_2013!B2</f>
+        <v>1.06</v>
       </c>
       <c r="C79" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="9">
+        <f>Serrenho_2013!B2</f>
+        <v>1.06</v>
+      </c>
+      <c r="C80" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="9">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B82" s="9">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C80" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
+      <c r="C82" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B81" s="9">
-        <v>1</v>
-      </c>
-      <c r="C81" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+      <c r="B83" s="9">
+        <v>1</v>
+      </c>
+      <c r="C83" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B84" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C82" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+      <c r="C84" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B85" s="9">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C83" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+      <c r="C85" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B84" s="9">
-        <v>1</v>
-      </c>
-      <c r="C84" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+      <c r="B86" s="9">
+        <v>1</v>
+      </c>
+      <c r="C86" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B87" s="9">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C85" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C87" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix column names in phi_constants table.
</commit_message>
<xml_diff>
--- a/inst/extdata/phi_constants.xlsx
+++ b/inst/extdata/phi_constants.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033FC482-708F-9D48-89D1-073F710F5691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49D41A8-C621-7B46-A58F-5756A9701C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24440" yWindow="1000" windowWidth="20020" windowHeight="27280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
   <si>
     <t>source</t>
   </si>
@@ -357,9 +357,6 @@
     <t>LTH.20.C</t>
   </si>
   <si>
-    <t>is.useful</t>
-  </si>
-  <si>
     <t>NEU</t>
   </si>
   <si>
@@ -367,6 +364,12 @@
   </si>
   <si>
     <t>Primary solid biofuels [from Resources]</t>
+  </si>
+  <si>
+    <t>IsUseful</t>
+  </si>
+  <si>
+    <t>PhiSource</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,20 +432,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -777,16 +773,15 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="5"/>
+    <col min="1" max="1" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -797,1210 +792,1210 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="b">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="b">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="b">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>0.95599999999999996</v>
       </c>
-      <c r="C5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9" t="b">
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <f>temp_calcs!G2</f>
         <v>0.8467020793849932</v>
       </c>
-      <c r="C7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <f>temp_calcs!G3</f>
         <v>0.81746813717700162</v>
       </c>
-      <c r="C8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="6">
         <f>temp_calcs!G4</f>
         <v>0.77445705533519227</v>
       </c>
-      <c r="C9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <f>temp_calcs!G5</f>
         <v>0.7671410615091433</v>
       </c>
-      <c r="C10" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <f>temp_calcs!G6</f>
         <v>0.74433512887860043</v>
       </c>
-      <c r="C11" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <f>temp_calcs!G7</f>
         <v>0.6711332531638321</v>
       </c>
-      <c r="C12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <f>temp_calcs!G8</f>
         <v>0.57342345688182428</v>
       </c>
-      <c r="C13" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <f>temp_calcs!G9</f>
         <v>0.49899677222367622</v>
       </c>
-      <c r="C14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <f>temp_calcs!G10</f>
         <v>0.39311000739723134</v>
       </c>
-      <c r="C15" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <f>temp_calcs!G11</f>
         <v>0.23047032024654968</v>
       </c>
-      <c r="C16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="6">
         <f>temp_calcs!G12</f>
         <v>0.13807594176797244</v>
       </c>
-      <c r="C17" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="6">
         <f>temp_calcs!G13</f>
         <v>5.116834385127067E-2</v>
       </c>
-      <c r="C18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="6">
         <f>temp_calcs!G14</f>
         <v>3.4112229234180447E-2</v>
       </c>
-      <c r="C19" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="6">
         <f>temp_calcs!G15</f>
         <v>0.114003420102603</v>
       </c>
-      <c r="C20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="b">
+      <c r="A21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C22" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C23" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C24" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="9">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9" t="b">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="9">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="b">
+      <c r="A26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9" t="b">
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C28" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C29" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C30" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C31" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C32" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C33" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C34" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="6">
         <f>Serrenho_2013!B4</f>
         <v>1.05</v>
       </c>
-      <c r="C35" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="6">
         <f>Serrenho_2013!B4</f>
         <v>1.05</v>
       </c>
-      <c r="C36" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="9">
-        <v>1</v>
-      </c>
-      <c r="C37" s="9" t="b">
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C38" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C39" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C40" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C41" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C42" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="C42" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="9" t="b">
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="9">
-        <v>1</v>
-      </c>
-      <c r="C44" s="9" t="b">
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
-      <c r="C45" s="9" t="b">
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C46" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C47" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="9">
+      <c r="A48" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="6">
         <f>Serrenho_2013!B7</f>
         <v>1</v>
       </c>
-      <c r="C48" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="6">
         <f>Serrenho_2013!B4</f>
         <v>1.05</v>
       </c>
-      <c r="C49" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C50" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="9">
-        <v>1</v>
-      </c>
-      <c r="C51" s="9" t="b">
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C52" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C53" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C54" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" s="4" t="s">
+      <c r="C54" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C55" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="9">
-        <v>1</v>
-      </c>
-      <c r="C56" s="9" t="b">
+      <c r="B56" s="6">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="6">
         <f>Serrenho_2013!B9</f>
         <v>0.6</v>
       </c>
-      <c r="C57" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="4" t="s">
+      <c r="C57" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C58" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="4" t="s">
+      <c r="C58" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="6">
         <f>Serrenho_2013!B9</f>
         <v>0.6</v>
       </c>
-      <c r="C59" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="C59" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="9">
-        <v>1</v>
-      </c>
-      <c r="C60" s="9" t="b">
+      <c r="B60" s="6">
+        <v>1</v>
+      </c>
+      <c r="C60" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C61" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="C61" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C62" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D62" s="4" t="s">
+      <c r="C62" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B63" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C63" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D63" s="4" t="s">
+      <c r="C63" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C64" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D64" s="4" t="s">
+      <c r="C64" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B65" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C65" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="C65" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C66" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D66" s="4" t="s">
+      <c r="C66" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="9">
-        <v>1</v>
-      </c>
-      <c r="C67" s="9" t="b">
+      <c r="B67" s="6">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="9">
-        <v>1</v>
-      </c>
-      <c r="C68" s="9" t="b">
+      <c r="B68" s="6">
+        <v>1</v>
+      </c>
+      <c r="C68" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C69" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="9">
+      <c r="B70" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C70" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D70" s="4" t="s">
+      <c r="C70" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="9">
-        <v>1</v>
-      </c>
-      <c r="C71" s="9" t="b">
+      <c r="B71" s="6">
+        <v>1</v>
+      </c>
+      <c r="C71" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="9">
-        <v>1</v>
-      </c>
-      <c r="C72" s="9" t="b">
+      <c r="B72" s="6">
+        <v>1</v>
+      </c>
+      <c r="C72" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C73" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D73" s="4" t="s">
+      <c r="C73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="6">
         <f>Serrenho_2013!B10</f>
         <v>0.25</v>
       </c>
-      <c r="C74" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D74" s="4" t="s">
+      <c r="C74" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C75" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D75" s="4" t="s">
+      <c r="C75" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C76" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D76" s="4" t="s">
+      <c r="C76" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="9">
+      <c r="B77" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C77" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D77" s="4" t="s">
+      <c r="C77" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B78" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C78" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D78" s="4" t="s">
+      <c r="C78" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B79" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C79" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D79" s="4" t="s">
+      <c r="C79" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B80" s="6">
         <f>Serrenho_2013!B2</f>
         <v>1.06</v>
       </c>
-      <c r="C80" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="C80" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="9">
-        <v>1</v>
-      </c>
-      <c r="C81" s="9" t="b">
+      <c r="B81" s="6">
+        <v>1</v>
+      </c>
+      <c r="C81" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B82" s="6">
         <f>Serrenho_2013!B5</f>
         <v>1.04</v>
       </c>
-      <c r="C82" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D82" s="4" t="s">
+      <c r="C82" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="9">
-        <v>1</v>
-      </c>
-      <c r="C83" s="9" t="b">
+      <c r="B83" s="6">
+        <v>1</v>
+      </c>
+      <c r="C83" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B84" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C84" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D84" s="4" t="s">
+      <c r="C84" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B85" s="6">
         <f>Serrenho_2013!B3</f>
         <v>1.06</v>
       </c>
-      <c r="C85" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="9">
-        <v>1</v>
-      </c>
-      <c r="C86" s="9" t="b">
+      <c r="B86" s="6">
+        <v>1</v>
+      </c>
+      <c r="C86" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="6">
         <f>Serrenho_2013!B6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="C87" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D87" s="4" t="s">
+      <c r="C87" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2052,7 +2047,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1">
@@ -2078,7 +2073,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1">
@@ -2104,7 +2099,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
@@ -2130,7 +2125,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
@@ -2156,7 +2151,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="1">
@@ -2182,7 +2177,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1">
@@ -2208,7 +2203,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
@@ -2234,7 +2229,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1">
@@ -2260,7 +2255,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1">
@@ -2286,7 +2281,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -2315,7 +2310,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1">
@@ -2341,7 +2336,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B13" s="1">
@@ -2370,7 +2365,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1">
@@ -2396,7 +2391,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1">

</xml_diff>